<commit_message>
Multiple contracts single file case hotfix
</commit_message>
<xml_diff>
--- a/contract_stats.xlsx
+++ b/contract_stats.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,7 +430,7 @@
         <v>EntryPositionsManager</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -450,7 +450,7 @@
         <v>ExitPositionsManager</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -470,10 +470,10 @@
         <v>IncentivesVault</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>7</v>
@@ -490,10 +490,10 @@
         <v>InterestRatesManager</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -507,7 +507,7 @@
         <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IAaveIncentivesController.sol</v>
       </c>
       <c r="B6" t="str">
-        <v>IAaveIncentivesController</v>
+        <v>IAaveDistributionManager</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -516,7 +516,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -524,19 +524,19 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IAToken.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IAaveIncentivesController.sol</v>
       </c>
       <c r="B7" t="str">
-        <v>IAToken</v>
+        <v>IAaveIncentivesController</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -544,10 +544,10 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IERC20.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IAToken.sol</v>
       </c>
       <c r="B8" t="str">
-        <v>IERC20</v>
+        <v>IAToken</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -564,19 +564,19 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\ILendingPool.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IERC20.sol</v>
       </c>
       <c r="B9" t="str">
-        <v>ILendingPool</v>
+        <v>IERC20</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -584,10 +584,10 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\ILendingPoolAddressesProvider.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\ILendingPool.sol</v>
       </c>
       <c r="B10" t="str">
-        <v>ILendingPoolAddressesProvider</v>
+        <v>ILendingPool</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -604,10 +604,10 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IPriceOracleGetter.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\ILendingPoolAddressesProvider.sol</v>
       </c>
       <c r="B11" t="str">
-        <v>IPriceOracleGetter</v>
+        <v>ILendingPoolAddressesProvider</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -616,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -624,10 +624,10 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IScaledBalanceToken.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IPriceOracleGetter.sol</v>
       </c>
       <c r="B12" t="str">
-        <v>IScaledBalanceToken</v>
+        <v>IPriceOracleGetter</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -636,7 +636,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -644,19 +644,19 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IVariableDebtToken.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IScaledBalanceToken.sol</v>
       </c>
       <c r="B13" t="str">
-        <v>IVariableDebtToken</v>
+        <v>IScaledBalanceToken</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -664,10 +664,10 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IEntryPositionsManager.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IVariableDebtToken.sol</v>
       </c>
       <c r="B14" t="str">
-        <v>IEntryPositionsManager</v>
+        <v>IVariableDebtToken</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -684,10 +684,10 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IExitPositionsManager.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IEntryPositionsManager.sol</v>
       </c>
       <c r="B15" t="str">
-        <v>IExitPositionsManager</v>
+        <v>IEntryPositionsManager</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -704,10 +704,10 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IGetterUnderlyingAsset.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IExitPositionsManager.sol</v>
       </c>
       <c r="B16" t="str">
-        <v>IGetterUnderlyingAsset</v>
+        <v>IExitPositionsManager</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -716,7 +716,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -724,19 +724,19 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IIncentivesVault.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IGetterUnderlyingAsset.sol</v>
       </c>
       <c r="B17" t="str">
-        <v>IIncentivesVault</v>
+        <v>IGetterUnderlyingAsset</v>
       </c>
       <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>1</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>11</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -744,10 +744,10 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IInterestRatesManager.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IIncentivesVault.sol</v>
       </c>
       <c r="B18" t="str">
-        <v>IInterestRatesManager</v>
+        <v>IIncentivesVault</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -756,7 +756,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -764,19 +764,19 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IMorpho.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IInterestRatesManager.sol</v>
       </c>
       <c r="B19" t="str">
-        <v>IMorpho</v>
+        <v>IInterestRatesManager</v>
       </c>
       <c r="C19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -784,10 +784,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IOracle.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IMorpho.sol</v>
       </c>
       <c r="B20" t="str">
-        <v>IOracle</v>
+        <v>IMorpho</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -796,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -804,19 +804,19 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IRewardsManager.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IOracle.sol</v>
       </c>
       <c r="B21" t="str">
-        <v>IRewardsManager</v>
+        <v>IOracle</v>
       </c>
       <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
         <v>1</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>5</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -824,10 +824,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\lido\ILido.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IRewardsManager.sol</v>
       </c>
       <c r="B22" t="str">
-        <v>ILido</v>
+        <v>IRewardsManager</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -836,7 +836,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -844,19 +844,19 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\IndexesLens.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\lido\ILido.sol</v>
       </c>
       <c r="B23" t="str">
-        <v>IndexesLens</v>
+        <v>ILido</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -864,19 +864,19 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\interfaces\ILens.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\lens\IndexesLens.sol</v>
       </c>
       <c r="B24" t="str">
-        <v>ILens</v>
+        <v>IndexesLens</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -884,19 +884,19 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\Lens.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\lens\interfaces\ILens.sol</v>
       </c>
       <c r="B25" t="str">
-        <v>Lens</v>
+        <v>ILens</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -904,53 +904,53 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\LensStorage.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\lens\Lens.sol</v>
       </c>
       <c r="B26" t="str">
-        <v>LensStorage</v>
+        <v>Lens</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
         <v>3</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
       <c r="F26">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\MarketsLens.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\lens\LensStorage.sol</v>
       </c>
       <c r="B27" t="str">
-        <v>MarketsLens</v>
+        <v>LensStorage</v>
       </c>
       <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
         <v>1</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>12</v>
-      </c>
       <c r="F27">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\RatesLens.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\lens\MarketsLens.sol</v>
       </c>
       <c r="B28" t="str">
-        <v>RatesLens</v>
+        <v>MarketsLens</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -964,19 +964,19 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\UsersLens.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\lens\RatesLens.sol</v>
       </c>
       <c r="B29" t="str">
-        <v>UsersLens</v>
+        <v>RatesLens</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -984,10 +984,10 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\DataTypes.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\lens\UsersLens.sol</v>
       </c>
       <c r="B30" t="str">
-        <v>DataTypes</v>
+        <v>UsersLens</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -996,7 +996,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1004,10 +1004,10 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\Errors.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\DataTypes.sol</v>
       </c>
       <c r="B31" t="str">
-        <v>Errors</v>
+        <v>DataTypes</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1019,64 +1019,64 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\ReserveConfiguration.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\Errors.sol</v>
       </c>
       <c r="B32" t="str">
-        <v>ReserveConfiguration</v>
+        <v>Errors</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>22</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\UserConfiguration.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\ReserveConfiguration.sol</v>
       </c>
       <c r="B33" t="str">
-        <v>UserConfiguration</v>
+        <v>ReserveConfiguration</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\InterestRatesModel.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\UserConfiguration.sol</v>
       </c>
       <c r="B34" t="str">
-        <v>InterestRatesModel</v>
+        <v>UserConfiguration</v>
       </c>
       <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
         <v>1</v>
-      </c>
-      <c r="D34">
-        <v>3</v>
-      </c>
-      <c r="E34">
-        <v>5</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\Types.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\libraries\InterestRatesModel.sol</v>
       </c>
       <c r="B35" t="str">
-        <v>Types</v>
+        <v>InterestRatesModel</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1096,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1104,19 +1104,19 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\MatchingEngine.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\libraries\Types.sol</v>
       </c>
       <c r="B36" t="str">
-        <v>MatchingEngine</v>
+        <v>Types</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1124,19 +1124,19 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\Morpho.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\MatchingEngine.sol</v>
       </c>
       <c r="B37" t="str">
-        <v>Morpho</v>
+        <v>MatchingEngine</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1144,19 +1144,19 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\MorphoGovernance.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\Morpho.sol</v>
       </c>
       <c r="B38" t="str">
-        <v>MorphoGovernance</v>
+        <v>Morpho</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1164,59 +1164,59 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\MorphoStorage.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\MorphoGovernance.sol</v>
       </c>
       <c r="B39" t="str">
-        <v>MorphoStorage</v>
+        <v>MorphoGovernance</v>
       </c>
       <c r="C39">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="F39">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\MorphoUtils.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\MorphoStorage.sol</v>
       </c>
       <c r="B40" t="str">
-        <v>MorphoUtils</v>
+        <v>MorphoStorage</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\PositionsManagerUtils.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\MorphoUtils.sol</v>
       </c>
       <c r="B41" t="str">
-        <v>PositionsManagerUtils</v>
+        <v>MorphoUtils</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1224,90 +1224,90 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>morpho\morpho-v1-main\src\common\rewards-distribution\RewardsDistributor.sol</v>
+        <v>morpho\morpho-v1-main\src\aave-v2\PositionsManagerUtils.sol</v>
       </c>
       <c r="B42" t="str">
-        <v>RewardsDistributor</v>
+        <v>PositionsManagerUtils</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E42">
         <v>4</v>
       </c>
       <c r="F42">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>morpho\morpho-v1-main\src\common\test\FakeToken.sol</v>
+        <v>morpho\morpho-v1-main\src\common\rewards-distribution\RewardsDistributor.sol</v>
       </c>
       <c r="B43" t="str">
-        <v>FakeToken</v>
+        <v>RewardsDistributor</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>morpho\morpho-v1-main\src\compound\IncentivesVault.sol</v>
+        <v>morpho\morpho-v1-main\src\common\test\FakeToken.sol</v>
       </c>
       <c r="B44" t="str">
-        <v>IncentivesVault</v>
+        <v>FakeToken</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F44">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>morpho\morpho-v1-main\src\compound\InterestRatesManager.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\IncentivesVault.sol</v>
       </c>
       <c r="B45" t="str">
-        <v>InterestRatesManager</v>
+        <v>IncentivesVault</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\compound\ICompound.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\InterestRatesManager.sol</v>
       </c>
       <c r="B46" t="str">
-        <v>ICompoundOracle</v>
+        <v>InterestRatesManager</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1316,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>106</v>
+        <v>2</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -1324,19 +1324,19 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IIncentivesVault.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\compound\ICompound.sol</v>
       </c>
       <c r="B47" t="str">
-        <v>IIncentivesVault</v>
+        <v>ICEth</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IInterestRatesManager.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\compound\ICompound.sol</v>
       </c>
       <c r="B48" t="str">
-        <v>IInterestRatesManager</v>
+        <v>IComptroller</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -1364,19 +1364,19 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IMorpho.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\compound\ICompound.sol</v>
       </c>
       <c r="B49" t="str">
-        <v>IMorpho</v>
+        <v>IInterestRateModel</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -1384,10 +1384,10 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IOracle.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\compound\ICompound.sol</v>
       </c>
       <c r="B50" t="str">
-        <v>IOracle</v>
+        <v>ICToken</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1396,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -1404,10 +1404,10 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IPositionsManager.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\compound\ICompound.sol</v>
       </c>
       <c r="B51" t="str">
-        <v>IPositionsManager</v>
+        <v>ICEther</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1416,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -1424,19 +1424,19 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IRewardsManager.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\compound\ICompound.sol</v>
       </c>
       <c r="B52" t="str">
-        <v>IRewardsManager</v>
+        <v>ICompoundOracle</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -1444,10 +1444,10 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IWETH.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\IIncentivesVault.sol</v>
       </c>
       <c r="B53" t="str">
-        <v>IWETH</v>
+        <v>IIncentivesVault</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1456,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -1464,19 +1464,19 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\IndexesLens.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\IInterestRatesManager.sol</v>
       </c>
       <c r="B54" t="str">
-        <v>IndexesLens</v>
+        <v>IInterestRatesManager</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -1484,19 +1484,19 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\interfaces\ILens.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\IMorpho.sol</v>
       </c>
       <c r="B55" t="str">
-        <v>ILens</v>
+        <v>IMorpho</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -1504,19 +1504,19 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\Lens.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\IOracle.sol</v>
       </c>
       <c r="B56" t="str">
-        <v>Lens</v>
+        <v>IOracle</v>
       </c>
       <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
         <v>1</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>3</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -1524,39 +1524,39 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\LensStorage.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\IPositionsManager.sol</v>
       </c>
       <c r="B57" t="str">
-        <v>LensStorage</v>
+        <v>IPositionsManager</v>
       </c>
       <c r="C57">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F57">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\MarketsLens.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\IRewardsManager.sol</v>
       </c>
       <c r="B58" t="str">
-        <v>MarketsLens</v>
+        <v>IRewardsManager</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -1564,19 +1564,19 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\RatesLens.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\interfaces\IWETH.sol</v>
       </c>
       <c r="B59" t="str">
-        <v>RatesLens</v>
+        <v>IWETH</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
       <c r="E59">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -1584,19 +1584,19 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\RewardsLens.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\lens\IndexesLens.sol</v>
       </c>
       <c r="B60" t="str">
-        <v>RewardsLens</v>
+        <v>IndexesLens</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -1604,19 +1604,19 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\UsersLens.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\lens\interfaces\ILens.sol</v>
       </c>
       <c r="B61" t="str">
-        <v>UsersLens</v>
+        <v>ILens</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
       <c r="E61">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -1624,10 +1624,10 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>morpho\morpho-v1-main\src\compound\libraries\CompoundMath.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\lens\Lens.sol</v>
       </c>
       <c r="B62" t="str">
-        <v>CompoundMath</v>
+        <v>Lens</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1636,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -1644,30 +1644,30 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>morpho\morpho-v1-main\src\compound\libraries\InterestRatesModel.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\lens\LensStorage.sol</v>
       </c>
       <c r="B63" t="str">
-        <v>InterestRatesModel</v>
+        <v>LensStorage</v>
       </c>
       <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
         <v>1</v>
       </c>
-      <c r="D63">
-        <v>3</v>
-      </c>
-      <c r="E63">
-        <v>5</v>
-      </c>
       <c r="F63">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>morpho\morpho-v1-main\src\compound\libraries\Types.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\lens\MarketsLens.sol</v>
       </c>
       <c r="B64" t="str">
-        <v>Types</v>
+        <v>MarketsLens</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1676,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -1684,19 +1684,19 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>morpho\morpho-v1-main\src\compound\MatchingEngine.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\lens\RatesLens.sol</v>
       </c>
       <c r="B65" t="str">
-        <v>MatchingEngine</v>
+        <v>RatesLens</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
       <c r="E65">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -1704,19 +1704,19 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>morpho\morpho-v1-main\src\compound\Morpho.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\lens\RewardsLens.sol</v>
       </c>
       <c r="B66" t="str">
-        <v>Morpho</v>
+        <v>RewardsLens</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -1724,19 +1724,19 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>morpho\morpho-v1-main\src\compound\MorphoGovernance.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\lens\UsersLens.sol</v>
       </c>
       <c r="B67" t="str">
-        <v>MorphoGovernance</v>
+        <v>UsersLens</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
       <c r="E67">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -1744,59 +1744,59 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>morpho\morpho-v1-main\src\compound\MorphoStorage.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\libraries\CompoundMath.sol</v>
       </c>
       <c r="B68" t="str">
-        <v>MorphoStorage</v>
+        <v>CompoundMath</v>
       </c>
       <c r="C68">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F68">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>morpho\morpho-v1-main\src\compound\MorphoUtils.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\libraries\InterestRatesModel.sol</v>
       </c>
       <c r="B69" t="str">
-        <v>MorphoUtils</v>
+        <v>InterestRatesModel</v>
       </c>
       <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>5</v>
+      </c>
+      <c r="F69">
         <v>2</v>
-      </c>
-      <c r="D69">
-        <v>3</v>
-      </c>
-      <c r="E69">
-        <v>11</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>morpho\morpho-v1-main\src\compound\PositionsManager.sol</v>
+        <v>morpho\morpho-v1-main\src\compound\libraries\Types.sol</v>
       </c>
       <c r="B70" t="str">
-        <v>PositionsManager</v>
+        <v>Types</v>
       </c>
       <c r="C70">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D70">
         <v>0</v>
       </c>
       <c r="E70">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -1804,27 +1804,147 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
+        <v>morpho\morpho-v1-main\src\compound\MatchingEngine.sol</v>
+      </c>
+      <c r="B71" t="str">
+        <v>MatchingEngine</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>6</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>morpho\morpho-v1-main\src\compound\Morpho.sol</v>
+      </c>
+      <c r="B72" t="str">
+        <v>Morpho</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>16</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>morpho\morpho-v1-main\src\compound\MorphoGovernance.sol</v>
+      </c>
+      <c r="B73" t="str">
+        <v>MorphoGovernance</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>25</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>morpho\morpho-v1-main\src\compound\MorphoStorage.sol</v>
+      </c>
+      <c r="B74" t="str">
+        <v>MorphoStorage</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>morpho\morpho-v1-main\src\compound\MorphoUtils.sol</v>
+      </c>
+      <c r="B75" t="str">
+        <v>MorphoUtils</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>11</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>morpho\morpho-v1-main\src\compound\PositionsManager.sol</v>
+      </c>
+      <c r="B76" t="str">
+        <v>PositionsManager</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>15</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
         <v>morpho\morpho-v1-main\src\compound\RewardsManager.sol</v>
       </c>
-      <c r="B71" t="str">
+      <c r="B77" t="str">
         <v>RewardsManager</v>
       </c>
-      <c r="C71">
-        <v>3</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-      <c r="E71">
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
         <v>12</v>
       </c>
-      <c r="F71">
+      <c r="F77">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F71"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F77"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Functionality for counting number of lines in each contract has been added
</commit_message>
<xml_diff>
--- a/contract_stats.xlsx
+++ b/contract_stats.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,6 +421,9 @@
       <c r="F1" t="str">
         <v>State Variables</v>
       </c>
+      <c r="G1" t="str">
+        <v>Number of lines</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -441,6 +444,9 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2">
+        <v>284</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -461,6 +467,9 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="G3">
+        <v>703</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -481,6 +490,9 @@
       <c r="F4">
         <v>8</v>
       </c>
+      <c r="G4">
+        <v>134</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -501,6 +513,9 @@
       <c r="F5">
         <v>0</v>
       </c>
+      <c r="G5">
+        <v>171</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -521,6 +536,9 @@
       <c r="F6">
         <v>0</v>
       </c>
+      <c r="G6">
+        <v>46</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -541,6 +559,9 @@
       <c r="F7">
         <v>0</v>
       </c>
+      <c r="G7">
+        <v>103</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -561,6 +582,9 @@
       <c r="F8">
         <v>0</v>
       </c>
+      <c r="G8">
+        <v>84</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -581,6 +605,9 @@
       <c r="F9">
         <v>0</v>
       </c>
+      <c r="G9">
+        <v>74</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -601,6 +628,9 @@
       <c r="F10">
         <v>0</v>
       </c>
+      <c r="G10">
+        <v>410</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -621,6 +651,9 @@
       <c r="F11">
         <v>0</v>
       </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -641,6 +674,9 @@
       <c r="F12">
         <v>0</v>
       </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -661,6 +697,9 @@
       <c r="F13">
         <v>0</v>
       </c>
+      <c r="G13">
+        <v>23</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -681,6 +720,9 @@
       <c r="F14">
         <v>0</v>
       </c>
+      <c r="G14">
+        <v>68</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -701,6 +743,9 @@
       <c r="F15">
         <v>0</v>
       </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -721,6 +766,9 @@
       <c r="F16">
         <v>0</v>
       </c>
+      <c r="G16">
+        <v>26</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -741,6 +789,9 @@
       <c r="F17">
         <v>0</v>
       </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -761,6 +812,9 @@
       <c r="F18">
         <v>0</v>
       </c>
+      <c r="G18">
+        <v>23</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -781,6 +835,9 @@
       <c r="F19">
         <v>0</v>
       </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -801,6 +858,9 @@
       <c r="F20">
         <v>0</v>
       </c>
+      <c r="G20">
+        <v>88</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -821,6 +881,9 @@
       <c r="F21">
         <v>0</v>
       </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -841,6 +904,9 @@
       <c r="F22">
         <v>0</v>
       </c>
+      <c r="G22">
+        <v>21</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -861,6 +927,9 @@
       <c r="F23">
         <v>0</v>
       </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -881,6 +950,9 @@
       <c r="F24">
         <v>0</v>
       </c>
+      <c r="G24">
+        <v>113</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -901,6 +973,9 @@
       <c r="F25">
         <v>0</v>
       </c>
+      <c r="G25">
+        <v>249</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -921,6 +996,9 @@
       <c r="F26">
         <v>0</v>
       </c>
+      <c r="G26">
+        <v>98</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -941,6 +1019,9 @@
       <c r="F27">
         <v>7</v>
       </c>
+      <c r="G27">
+        <v>29</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -961,6 +1042,9 @@
       <c r="F28">
         <v>0</v>
       </c>
+      <c r="G28">
+        <v>225</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -981,6 +1065,9 @@
       <c r="F29">
         <v>0</v>
       </c>
+      <c r="G29">
+        <v>457</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1001,6 +1088,9 @@
       <c r="F30">
         <v>0</v>
       </c>
+      <c r="G30">
+        <v>471</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1021,6 +1111,9 @@
       <c r="F31">
         <v>0</v>
       </c>
+      <c r="G31">
+        <v>50</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1041,6 +1134,9 @@
       <c r="F32">
         <v>80</v>
       </c>
+      <c r="G32">
+        <v>98</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1061,6 +1157,9 @@
       <c r="F33">
         <v>22</v>
       </c>
+      <c r="G33">
+        <v>364</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -1081,6 +1180,9 @@
       <c r="F34">
         <v>0</v>
       </c>
+      <c r="G34">
+        <v>11</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -1101,6 +1203,9 @@
       <c r="F35">
         <v>0</v>
       </c>
+      <c r="G35">
+        <v>197</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1121,6 +1226,9 @@
       <c r="F36">
         <v>0</v>
       </c>
+      <c r="G36">
+        <v>97</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1141,6 +1249,9 @@
       <c r="F37">
         <v>0</v>
       </c>
+      <c r="G37">
+        <v>344</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1161,6 +1272,9 @@
       <c r="F38">
         <v>0</v>
       </c>
+      <c r="G38">
+        <v>235</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1181,6 +1295,9 @@
       <c r="F39">
         <v>0</v>
       </c>
+      <c r="G39">
+        <v>519</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1201,6 +1318,9 @@
       <c r="F40">
         <v>37</v>
       </c>
+      <c r="G40">
+        <v>66</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -1221,6 +1341,9 @@
       <c r="F41">
         <v>0</v>
       </c>
+      <c r="G41">
+        <v>317</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -1241,6 +1364,9 @@
       <c r="F42">
         <v>0</v>
       </c>
+      <c r="G42">
+        <v>86</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -1261,6 +1387,9 @@
       <c r="F43">
         <v>4</v>
       </c>
+      <c r="G43">
+        <v>91</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -1281,6 +1410,9 @@
       <c r="F44">
         <v>0</v>
       </c>
+      <c r="G44">
+        <v>7</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -1301,6 +1433,9 @@
       <c r="F45">
         <v>8</v>
       </c>
+      <c r="G45">
+        <v>139</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -1321,6 +1456,9 @@
       <c r="F46">
         <v>0</v>
       </c>
+      <c r="G46">
+        <v>155</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -1341,6 +1479,9 @@
       <c r="F47">
         <v>0</v>
       </c>
+      <c r="G47">
+        <v>43</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -1361,6 +1502,9 @@
       <c r="F48">
         <v>0</v>
       </c>
+      <c r="G48">
+        <v>203</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -1381,6 +1525,9 @@
       <c r="F49">
         <v>0</v>
       </c>
+      <c r="G49">
+        <v>14</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -1401,6 +1548,9 @@
       <c r="F50">
         <v>0</v>
       </c>
+      <c r="G50">
+        <v>103</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -1421,6 +1571,9 @@
       <c r="F51">
         <v>0</v>
       </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -1441,6 +1594,9 @@
       <c r="F52">
         <v>0</v>
       </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -1461,6 +1617,9 @@
       <c r="F53">
         <v>0</v>
       </c>
+      <c r="G53">
+        <v>23</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -1481,6 +1640,9 @@
       <c r="F54">
         <v>0</v>
       </c>
+      <c r="G54">
+        <v>3</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -1501,6 +1663,9 @@
       <c r="F55">
         <v>0</v>
       </c>
+      <c r="G55">
+        <v>76</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -1521,6 +1686,9 @@
       <c r="F56">
         <v>0</v>
       </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -1541,6 +1709,9 @@
       <c r="F57">
         <v>0</v>
       </c>
+      <c r="G57">
+        <v>40</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -1561,6 +1732,9 @@
       <c r="F58">
         <v>0</v>
       </c>
+      <c r="G58">
+        <v>33</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -1581,6 +1755,9 @@
       <c r="F59">
         <v>0</v>
       </c>
+      <c r="G59">
+        <v>5</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -1601,6 +1778,9 @@
       <c r="F60">
         <v>0</v>
       </c>
+      <c r="G60">
+        <v>147</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -1621,6 +1801,9 @@
       <c r="F61">
         <v>0</v>
       </c>
+      <c r="G61">
+        <v>283</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -1641,6 +1824,9 @@
       <c r="F62">
         <v>0</v>
       </c>
+      <c r="G62">
+        <v>87</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -1661,6 +1847,9 @@
       <c r="F63">
         <v>8</v>
       </c>
+      <c r="G63">
+        <v>28</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
@@ -1681,6 +1870,9 @@
       <c r="F64">
         <v>0</v>
       </c>
+      <c r="G64">
+        <v>170</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -1701,6 +1893,9 @@
       <c r="F65">
         <v>0</v>
       </c>
+      <c r="G65">
+        <v>443</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -1721,6 +1916,9 @@
       <c r="F66">
         <v>0</v>
       </c>
+      <c r="G66">
+        <v>171</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -1741,6 +1939,9 @@
       <c r="F67">
         <v>0</v>
       </c>
+      <c r="G67">
+        <v>461</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -1761,6 +1962,9 @@
       <c r="F68">
         <v>0</v>
       </c>
+      <c r="G68">
+        <v>45</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -1781,6 +1985,9 @@
       <c r="F69">
         <v>2</v>
       </c>
+      <c r="G69">
+        <v>194</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -1801,6 +2008,9 @@
       <c r="F70">
         <v>0</v>
       </c>
+      <c r="G70">
+        <v>86</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -1821,6 +2031,9 @@
       <c r="F71">
         <v>0</v>
       </c>
+      <c r="G71">
+        <v>376</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
@@ -1841,6 +2054,9 @@
       <c r="F72">
         <v>0</v>
       </c>
+      <c r="G72">
+        <v>237</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
@@ -1861,6 +2077,9 @@
       <c r="F73">
         <v>0</v>
       </c>
+      <c r="G73">
+        <v>477</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
@@ -1881,6 +2100,9 @@
       <c r="F74">
         <v>33</v>
       </c>
+      <c r="G74">
+        <v>56</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -1901,6 +2123,9 @@
       <c r="F75">
         <v>0</v>
       </c>
+      <c r="G75">
+        <v>212</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -1921,6 +2146,9 @@
       <c r="F76">
         <v>0</v>
       </c>
+      <c r="G76">
+        <v>1019</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -1941,10 +2169,13 @@
       <c r="F77">
         <v>7</v>
       </c>
+      <c r="G77">
+        <v>247</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F77"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G77"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More metrics for each contract has been added
</commit_message>
<xml_diff>
--- a/contract_stats.xlsx
+++ b/contract_stats.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,6 +424,21 @@
       <c r="G1" t="str">
         <v>Number of lines</v>
       </c>
+      <c r="H1" t="str">
+        <v>Number of structs</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Number of using-for</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Number of custom error definitions</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Number of events</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Number of inherited classes</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -447,6 +462,21 @@
       <c r="G2">
         <v>284</v>
       </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -470,6 +500,21 @@
       <c r="G3">
         <v>703</v>
       </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -493,6 +538,21 @@
       <c r="G4">
         <v>134</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -516,6 +576,21 @@
       <c r="G5">
         <v>171</v>
       </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -539,6 +614,21 @@
       <c r="G6">
         <v>46</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -562,6 +652,21 @@
       <c r="G7">
         <v>103</v>
       </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -585,6 +690,21 @@
       <c r="G8">
         <v>84</v>
       </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -608,6 +728,21 @@
       <c r="G9">
         <v>74</v>
       </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -631,6 +766,21 @@
       <c r="G10">
         <v>410</v>
       </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>13</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -654,6 +804,21 @@
       <c r="G11">
         <v>50</v>
       </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -677,6 +842,21 @@
       <c r="G12">
         <v>6</v>
       </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -700,6 +880,21 @@
       <c r="G13">
         <v>23</v>
       </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -723,6 +918,21 @@
       <c r="G14">
         <v>68</v>
       </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -746,6 +956,21 @@
       <c r="G15">
         <v>15</v>
       </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -769,6 +994,21 @@
       <c r="G16">
         <v>26</v>
       </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -792,6 +1032,21 @@
       <c r="G17">
         <v>3</v>
       </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -815,6 +1070,21 @@
       <c r="G18">
         <v>23</v>
       </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -838,6 +1108,21 @@
       <c r="G19">
         <v>3</v>
       </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -861,6 +1146,21 @@
       <c r="G20">
         <v>88</v>
       </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -884,6 +1184,21 @@
       <c r="G21">
         <v>3</v>
       </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -907,6 +1222,21 @@
       <c r="G22">
         <v>21</v>
       </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -930,6 +1260,21 @@
       <c r="G23">
         <v>5</v>
       </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -953,6 +1298,21 @@
       <c r="G24">
         <v>113</v>
       </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -976,6 +1336,21 @@
       <c r="G25">
         <v>249</v>
       </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -999,6 +1374,21 @@
       <c r="G26">
         <v>98</v>
       </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -1022,6 +1412,21 @@
       <c r="G27">
         <v>29</v>
       </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -1045,6 +1450,21 @@
       <c r="G28">
         <v>225</v>
       </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -1068,6 +1488,21 @@
       <c r="G29">
         <v>457</v>
       </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1091,6 +1526,21 @@
       <c r="G30">
         <v>471</v>
       </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1114,6 +1564,21 @@
       <c r="G31">
         <v>50</v>
       </c>
+      <c r="H31">
+        <v>3</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1137,6 +1602,21 @@
       <c r="G32">
         <v>98</v>
       </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1160,6 +1640,21 @@
       <c r="G33">
         <v>364</v>
       </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -1183,6 +1678,21 @@
       <c r="G34">
         <v>11</v>
       </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -1206,6 +1716,21 @@
       <c r="G35">
         <v>197</v>
       </c>
+      <c r="H35">
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1229,6 +1754,21 @@
       <c r="G36">
         <v>97</v>
       </c>
+      <c r="H36">
+        <v>11</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1252,6 +1792,21 @@
       <c r="G37">
         <v>344</v>
       </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1275,6 +1830,21 @@
       <c r="G38">
         <v>235</v>
       </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1298,6 +1868,21 @@
       <c r="G39">
         <v>519</v>
       </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+      <c r="J39">
+        <v>6</v>
+      </c>
+      <c r="K39">
+        <v>22</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1321,6 +1906,21 @@
       <c r="G40">
         <v>66</v>
       </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>2</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -1344,6 +1944,21 @@
       <c r="G41">
         <v>317</v>
       </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>7</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -1367,6 +1982,21 @@
       <c r="G42">
         <v>86</v>
       </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42">
+        <v>3</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -1390,6 +2020,21 @@
       <c r="G43">
         <v>91</v>
       </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+      <c r="K43">
+        <v>3</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -1413,6 +2058,21 @@
       <c r="G44">
         <v>7</v>
       </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -1436,6 +2096,21 @@
       <c r="G45">
         <v>139</v>
       </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+      <c r="K45">
+        <v>6</v>
+      </c>
+      <c r="L45">
+        <v>2</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -1459,6 +2134,21 @@
       <c r="G46">
         <v>155</v>
       </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>2</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>2</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -1482,6 +2172,21 @@
       <c r="G47">
         <v>43</v>
       </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -1505,6 +2210,21 @@
       <c r="G48">
         <v>203</v>
       </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -1528,6 +2248,21 @@
       <c r="G49">
         <v>14</v>
       </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -1551,6 +2286,21 @@
       <c r="G50">
         <v>103</v>
       </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -1574,6 +2324,21 @@
       <c r="G51">
         <v>5</v>
       </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -1597,6 +2362,21 @@
       <c r="G52">
         <v>3</v>
       </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -1620,6 +2400,21 @@
       <c r="G53">
         <v>23</v>
       </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -1643,6 +2438,21 @@
       <c r="G54">
         <v>3</v>
       </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -1666,6 +2476,21 @@
       <c r="G55">
         <v>76</v>
       </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -1689,6 +2514,21 @@
       <c r="G56">
         <v>3</v>
       </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -1712,6 +2552,21 @@
       <c r="G57">
         <v>40</v>
       </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -1735,6 +2590,21 @@
       <c r="G58">
         <v>33</v>
       </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -1758,6 +2628,21 @@
       <c r="G59">
         <v>5</v>
       </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -1781,6 +2666,21 @@
       <c r="G60">
         <v>147</v>
       </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -1804,6 +2704,21 @@
       <c r="G61">
         <v>283</v>
       </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -1827,6 +2742,21 @@
       <c r="G62">
         <v>87</v>
       </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -1850,6 +2780,21 @@
       <c r="G63">
         <v>28</v>
       </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>2</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
@@ -1873,6 +2818,21 @@
       <c r="G64">
         <v>170</v>
       </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -1896,6 +2856,21 @@
       <c r="G65">
         <v>443</v>
       </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>2</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -1919,6 +2894,21 @@
       <c r="G66">
         <v>171</v>
       </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -1942,6 +2932,21 @@
       <c r="G67">
         <v>461</v>
       </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>2</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -1965,6 +2970,21 @@
       <c r="G68">
         <v>45</v>
       </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>2</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -1988,6 +3008,21 @@
       <c r="G69">
         <v>194</v>
       </c>
+      <c r="H69">
+        <v>4</v>
+      </c>
+      <c r="I69">
+        <v>2</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -2011,6 +3046,21 @@
       <c r="G70">
         <v>86</v>
       </c>
+      <c r="H70">
+        <v>11</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -2034,6 +3084,21 @@
       <c r="G71">
         <v>376</v>
       </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71">
+        <v>2</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>2</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
@@ -2057,6 +3122,21 @@
       <c r="G72">
         <v>237</v>
       </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>2</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
@@ -2080,6 +3160,21 @@
       <c r="G73">
         <v>477</v>
       </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>2</v>
+      </c>
+      <c r="J73">
+        <v>5</v>
+      </c>
+      <c r="K73">
+        <v>21</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
@@ -2103,6 +3198,21 @@
       <c r="G74">
         <v>56</v>
       </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>2</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -2126,6 +3236,21 @@
       <c r="G75">
         <v>212</v>
       </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>3</v>
+      </c>
+      <c r="J75">
+        <v>2</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -2149,6 +3274,21 @@
       <c r="G76">
         <v>1019</v>
       </c>
+      <c r="H76">
+        <v>4</v>
+      </c>
+      <c r="I76">
+        <v>3</v>
+      </c>
+      <c r="J76">
+        <v>19</v>
+      </c>
+      <c r="K76">
+        <v>9</v>
+      </c>
+      <c r="L76">
+        <v>2</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -2172,10 +3312,25 @@
       <c r="G77">
         <v>247</v>
       </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>2</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G77"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L77"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>